<commit_message>
stl for config design
</commit_message>
<xml_diff>
--- a/Product Manufacturing Information/Product Manufacturing Information - UAS-X1V1.xlsx
+++ b/Product Manufacturing Information/Product Manufacturing Information - UAS-X1V1.xlsx
@@ -477,6 +477,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -484,12 +490,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -774,8 +774,8 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -787,7 +787,7 @@
     <col min="5" max="5" width="25.21875" style="10" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="26.77734375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="45.21875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="45.21875" style="14" customWidth="1"/>
     <col min="9" max="13" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -826,7 +826,7 @@
       <c r="A2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -836,13 +836,13 @@
       <c r="E2" s="11"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="16"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="8" t="s">
         <v>91</v>
       </c>
@@ -850,13 +850,13 @@
       <c r="E3" s="11"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="16"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="8" t="s">
         <v>99</v>
       </c>
@@ -864,13 +864,13 @@
       <c r="E4" s="11"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="16"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="8" t="s">
         <v>92</v>
       </c>
@@ -878,13 +878,13 @@
       <c r="E5" s="11"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="16"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="8" t="s">
         <v>93</v>
       </c>
@@ -892,13 +892,13 @@
       <c r="E6" s="11"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="16"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="8" t="s">
         <v>100</v>
       </c>
@@ -906,13 +906,13 @@
       <c r="E7" s="11"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="16"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="8" t="s">
         <v>94</v>
       </c>
@@ -920,13 +920,13 @@
       <c r="E8" s="11"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="8" t="s">
         <v>95</v>
       </c>
@@ -934,13 +934,13 @@
       <c r="E9" s="11"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="16"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="8" t="s">
         <v>96</v>
       </c>
@@ -948,13 +948,13 @@
       <c r="E10" s="11"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="16"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="15"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="8" t="s">
         <v>97</v>
       </c>
@@ -962,13 +962,13 @@
       <c r="E11" s="11"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="16"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="15"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="8" t="s">
         <v>101</v>
       </c>
@@ -976,13 +976,13 @@
       <c r="E12" s="11"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="16"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="15"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="8" t="s">
         <v>104</v>
       </c>
@@ -990,13 +990,13 @@
       <c r="E13" s="11"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="16"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -1006,13 +1006,15 @@
       <c r="E14" s="11"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="16"/>
+      <c r="H14" s="13">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="15"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="8" t="s">
         <v>52</v>
       </c>
@@ -1020,7 +1022,7 @@
       <c r="E15" s="11"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="16">
+      <c r="H15" s="13">
         <v>160</v>
       </c>
     </row>
@@ -1028,7 +1030,7 @@
       <c r="A16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="15"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="8" t="s">
         <v>53</v>
       </c>
@@ -1036,7 +1038,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="16">
+      <c r="H16" s="13">
         <v>50</v>
       </c>
     </row>
@@ -1044,7 +1046,7 @@
       <c r="A17" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="15"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="8" t="s">
         <v>54</v>
       </c>
@@ -1052,13 +1054,13 @@
       <c r="E17" s="11"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="16"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="15"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="8" t="s">
         <v>55</v>
       </c>
@@ -1066,13 +1068,13 @@
       <c r="E18" s="11"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="16"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="15"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="8" t="s">
         <v>56</v>
       </c>
@@ -1080,13 +1082,13 @@
       <c r="E19" s="11"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="16"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="15"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="8" t="s">
         <v>57</v>
       </c>
@@ -1094,13 +1096,13 @@
       <c r="E20" s="11"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="16"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="15"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="8" t="s">
         <v>58</v>
       </c>
@@ -1108,13 +1110,13 @@
       <c r="E21" s="11"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="16"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="15"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="8" t="s">
         <v>59</v>
       </c>
@@ -1122,13 +1124,13 @@
       <c r="E22" s="11"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="16"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="15"/>
+      <c r="B23" s="17"/>
       <c r="C23" s="8" t="s">
         <v>60</v>
       </c>
@@ -1136,13 +1138,13 @@
       <c r="E23" s="11"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="16"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="15"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="8" t="s">
         <v>61</v>
       </c>
@@ -1150,13 +1152,13 @@
       <c r="E24" s="11"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="16"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="8" t="s">
         <v>62</v>
       </c>
@@ -1164,13 +1166,13 @@
       <c r="E25" s="11"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="16"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="8" t="s">
         <v>63</v>
       </c>
@@ -1178,13 +1180,13 @@
       <c r="E26" s="11"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="16"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" s="17"/>
       <c r="C27" s="8" t="s">
         <v>64</v>
       </c>
@@ -1192,13 +1194,13 @@
       <c r="E27" s="11"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="16"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="15"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="8" t="s">
         <v>65</v>
       </c>
@@ -1206,13 +1208,13 @@
       <c r="E28" s="11"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="16"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="15"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="8" t="s">
         <v>66</v>
       </c>
@@ -1220,13 +1222,13 @@
       <c r="E29" s="11"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="16"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="15"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="8" t="s">
         <v>67</v>
       </c>
@@ -1234,13 +1236,13 @@
       <c r="E30" s="11"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="16"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="15"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="8" t="s">
         <v>68</v>
       </c>
@@ -1248,13 +1250,13 @@
       <c r="E31" s="11"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="16"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="15"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="8" t="s">
         <v>20</v>
       </c>
@@ -1264,13 +1266,13 @@
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="16"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="15"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="8" t="s">
         <v>11</v>
       </c>
@@ -1280,13 +1282,13 @@
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="16"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="15"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="8" t="s">
         <v>12</v>
       </c>
@@ -1296,13 +1298,13 @@
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="16"/>
+      <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="15"/>
+      <c r="B35" s="17"/>
       <c r="C35" s="8" t="s">
         <v>9</v>
       </c>
@@ -1312,13 +1314,13 @@
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="16"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="15"/>
+      <c r="B36" s="17"/>
       <c r="C36" s="8" t="s">
         <v>13</v>
       </c>
@@ -1328,13 +1330,13 @@
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="16"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="15"/>
+      <c r="B37" s="17"/>
       <c r="C37" s="8" t="s">
         <v>1</v>
       </c>
@@ -1344,13 +1346,13 @@
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
-      <c r="H37" s="16"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="15"/>
+      <c r="B38" s="17"/>
       <c r="C38" s="8" t="s">
         <v>0</v>
       </c>
@@ -1358,13 +1360,13 @@
       <c r="E38" s="11"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
-      <c r="H38" s="16"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="15"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="8" t="s">
         <v>2</v>
       </c>
@@ -1372,13 +1374,13 @@
       <c r="E39" s="11"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="16"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="15"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="8" t="s">
         <v>3</v>
       </c>
@@ -1388,13 +1390,13 @@
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="16"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="15"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="8" t="s">
         <v>4</v>
       </c>
@@ -1404,13 +1406,13 @@
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="16"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="15"/>
+      <c r="B42" s="17"/>
       <c r="C42" s="8" t="s">
         <v>10</v>
       </c>
@@ -1420,13 +1422,13 @@
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="16"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="15"/>
+      <c r="B43" s="17"/>
       <c r="C43" s="8" t="s">
         <v>5</v>
       </c>
@@ -1436,13 +1438,13 @@
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="16"/>
+      <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="15"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="8" t="s">
         <v>6</v>
       </c>
@@ -1452,13 +1454,13 @@
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="16"/>
+      <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="15"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="8" t="s">
         <v>7</v>
       </c>
@@ -1468,13 +1470,13 @@
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="16"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="15"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="8" t="s">
         <v>98</v>
       </c>
@@ -1484,13 +1486,13 @@
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="16"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="15" t="s">
         <v>106</v>
       </c>
       <c r="C47" s="8" t="s">
@@ -1500,13 +1502,13 @@
       <c r="E47" s="11"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="16"/>
+      <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="13"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="8" t="s">
         <v>15</v>
       </c>
@@ -1514,13 +1516,13 @@
       <c r="E48" s="11"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="16"/>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="13"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="8" t="s">
         <v>16</v>
       </c>
@@ -1528,7 +1530,7 @@
       <c r="E49" s="11"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="16"/>
+      <c r="H49" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>